<commit_message>
updated files Jul 21 - R and reports.
</commit_message>
<xml_diff>
--- a/data/Broad Drugs Reclassification.xlsx
+++ b/data/Broad Drugs Reclassification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deisygysi/Desktop/PostDoc/00_Projects/COVID19/BU_Prepare_Code_to_Submission/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deisygysi/Dropbox (CCNR)/BU_Paper_COVID/code/COVID19/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FF8CB08-BA35-0F49-963B-C37FB8A2BC34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0E2052-1EF5-0E46-B450-1D7228E3F80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{4D209F0B-E198-4676-AE8C-C8197309096E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="119">
   <si>
     <t>BIX-01294</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>Golgicide-A</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -473,12 +476,21 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -487,18 +499,149 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -509,6 +652,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B0D8AA06-16B9-B64D-8EE9-9B02DB9E1FBF}" name="Table2" displayName="Table2" ref="A1:F28" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="7">
+  <autoFilter ref="A1:F28" xr:uid="{20782B7B-AFB2-084F-99B7-D21934F4ED1C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
+    <sortCondition ref="A1:A28"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{0F1FE8B5-8FE0-CD40-8E57-61B067692E42}" name="Drug" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{B14B053E-0F27-8A49-A0AE-FCE865AA6919}" name="BRD Code" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{D42D7FEC-391A-DE4E-860F-FD25A8CF1042}" name="Master Plate" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9A748FFF-AB6E-D94A-9B64-E5A6AA395EE7}" name="Broad Plate" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{2CC043C0-A94B-8E47-BB68-2CF8DB456394}" name="Note" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{BD2B5768-767F-8841-90D6-AAE29DF0B529}" name="Category" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -811,7 +972,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -821,10 +982,11 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="116" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -839,372 +1001,372 @@
       <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
+      <c r="A2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
+      <c r="A3" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
+      <c r="A4" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="F17" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
+      <c r="A19" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1219,179 +1381,185 @@
       <c r="E20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>86</v>
+      <c r="A26" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>88</v>
+      <c r="A27" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>89</v>
+      <c r="A28" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1606,19 +1774,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8D1759-8BFC-41B3-BD42-39D40B1A7276}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBA9C0A3-9D9E-40D7-BE61-88F25DBE1870}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1643,9 +1807,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBA9C0A3-9D9E-40D7-BE61-88F25DBE1870}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8D1759-8BFC-41B3-BD42-39D40B1A7276}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>